<commit_message>
:sparkles: refactor client services
</commit_message>
<xml_diff>
--- a/api/utils/templates/xlsx/baseSigoSales.xlsx
+++ b/api/utils/templates/xlsx/baseSigoSales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\workspace\max-import-backend\api\utils\templates\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EA8154B0-25C8-46E9-B6F6-148E76AC193F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5306AE9-BD2A-416F-A8D2-B2CA5BA30A7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -951,7 +951,7 @@
     <numFmt numFmtId="165" formatCode="##,##0.00_);[Red]\(##,##0.00\)"/>
     <numFmt numFmtId="166" formatCode="##,##0.00000_);[Red]\(##,##0.00000\)"/>
   </numFmts>
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1146,13 +1146,6 @@
     </font>
     <font>
       <b/>
-      <u/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
       <u/>
       <sz val="10"/>
       <color theme="1"/>
@@ -1559,7 +1552,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1576,7 +1569,6 @@
     <xf numFmtId="0" fontId="26" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="26" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="26" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1959,11 +1951,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BA18"/>
+  <dimension ref="A1:BA5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA6" sqref="AA6"/>
+      <selection pane="bottomLeft" activeCell="AA5" sqref="AA5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -2025,230 +2017,230 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" ht="14.4" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
-      <c r="V1" s="18"/>
-      <c r="W1" s="18"/>
-      <c r="X1" s="18"/>
-      <c r="Y1" s="18"/>
-      <c r="Z1" s="18"/>
-      <c r="AA1" s="18"/>
-      <c r="AB1" s="18"/>
-      <c r="AC1" s="18"/>
-      <c r="AD1" s="18"/>
-      <c r="AE1" s="18"/>
-      <c r="AF1" s="18"/>
-      <c r="AG1" s="18"/>
-      <c r="AH1" s="18"/>
-      <c r="AI1" s="18"/>
-      <c r="AJ1" s="18"/>
-      <c r="AK1" s="18"/>
-      <c r="AL1" s="18"/>
-      <c r="AM1" s="18"/>
-      <c r="AN1" s="18"/>
-      <c r="AO1" s="18"/>
-      <c r="AP1" s="18"/>
-      <c r="AQ1" s="18"/>
-      <c r="AR1" s="18"/>
-      <c r="AS1" s="18"/>
-      <c r="AT1" s="18"/>
-      <c r="AU1" s="18"/>
-      <c r="AV1" s="18"/>
-      <c r="AW1" s="18"/>
-      <c r="AX1" s="18"/>
-      <c r="AY1" s="18"/>
-      <c r="AZ1" s="18"/>
-      <c r="BA1" s="18"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
+      <c r="W1" s="17"/>
+      <c r="X1" s="17"/>
+      <c r="Y1" s="17"/>
+      <c r="Z1" s="17"/>
+      <c r="AA1" s="17"/>
+      <c r="AB1" s="17"/>
+      <c r="AC1" s="17"/>
+      <c r="AD1" s="17"/>
+      <c r="AE1" s="17"/>
+      <c r="AF1" s="17"/>
+      <c r="AG1" s="17"/>
+      <c r="AH1" s="17"/>
+      <c r="AI1" s="17"/>
+      <c r="AJ1" s="17"/>
+      <c r="AK1" s="17"/>
+      <c r="AL1" s="17"/>
+      <c r="AM1" s="17"/>
+      <c r="AN1" s="17"/>
+      <c r="AO1" s="17"/>
+      <c r="AP1" s="17"/>
+      <c r="AQ1" s="17"/>
+      <c r="AR1" s="17"/>
+      <c r="AS1" s="17"/>
+      <c r="AT1" s="17"/>
+      <c r="AU1" s="17"/>
+      <c r="AV1" s="17"/>
+      <c r="AW1" s="17"/>
+      <c r="AX1" s="17"/>
+      <c r="AY1" s="17"/>
+      <c r="AZ1" s="17"/>
+      <c r="BA1" s="17"/>
     </row>
     <row r="2" spans="1:53" ht="23.4" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
-      <c r="T2" s="20"/>
-      <c r="U2" s="20"/>
-      <c r="V2" s="20"/>
-      <c r="W2" s="20"/>
-      <c r="X2" s="20"/>
-      <c r="Y2" s="20"/>
-      <c r="Z2" s="20"/>
-      <c r="AA2" s="20"/>
-      <c r="AB2" s="20"/>
-      <c r="AC2" s="20"/>
-      <c r="AD2" s="20"/>
-      <c r="AE2" s="20"/>
-      <c r="AF2" s="20"/>
-      <c r="AG2" s="20"/>
-      <c r="AH2" s="20"/>
-      <c r="AI2" s="20"/>
-      <c r="AJ2" s="20"/>
-      <c r="AK2" s="20"/>
-      <c r="AL2" s="20"/>
-      <c r="AM2" s="20"/>
-      <c r="AN2" s="20"/>
-      <c r="AO2" s="20"/>
-      <c r="AP2" s="20"/>
-      <c r="AQ2" s="20"/>
-      <c r="AR2" s="20"/>
-      <c r="AS2" s="20"/>
-      <c r="AT2" s="20"/>
-      <c r="AU2" s="20"/>
-      <c r="AV2" s="20"/>
-      <c r="AW2" s="20"/>
-      <c r="AX2" s="20"/>
-      <c r="AY2" s="20"/>
-      <c r="AZ2" s="20"/>
-      <c r="BA2" s="21"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
+      <c r="V2" s="19"/>
+      <c r="W2" s="19"/>
+      <c r="X2" s="19"/>
+      <c r="Y2" s="19"/>
+      <c r="Z2" s="19"/>
+      <c r="AA2" s="19"/>
+      <c r="AB2" s="19"/>
+      <c r="AC2" s="19"/>
+      <c r="AD2" s="19"/>
+      <c r="AE2" s="19"/>
+      <c r="AF2" s="19"/>
+      <c r="AG2" s="19"/>
+      <c r="AH2" s="19"/>
+      <c r="AI2" s="19"/>
+      <c r="AJ2" s="19"/>
+      <c r="AK2" s="19"/>
+      <c r="AL2" s="19"/>
+      <c r="AM2" s="19"/>
+      <c r="AN2" s="19"/>
+      <c r="AO2" s="19"/>
+      <c r="AP2" s="19"/>
+      <c r="AQ2" s="19"/>
+      <c r="AR2" s="19"/>
+      <c r="AS2" s="19"/>
+      <c r="AT2" s="19"/>
+      <c r="AU2" s="19"/>
+      <c r="AV2" s="19"/>
+      <c r="AW2" s="19"/>
+      <c r="AX2" s="19"/>
+      <c r="AY2" s="19"/>
+      <c r="AZ2" s="19"/>
+      <c r="BA2" s="20"/>
     </row>
     <row r="3" spans="1:53" ht="13.8" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="23"/>
-      <c r="O3" s="23"/>
-      <c r="P3" s="23"/>
-      <c r="Q3" s="23"/>
-      <c r="R3" s="23"/>
-      <c r="S3" s="23"/>
-      <c r="T3" s="23"/>
-      <c r="U3" s="23"/>
-      <c r="V3" s="23"/>
-      <c r="W3" s="23"/>
-      <c r="X3" s="23"/>
-      <c r="Y3" s="23"/>
-      <c r="Z3" s="23"/>
-      <c r="AA3" s="23"/>
-      <c r="AB3" s="23"/>
-      <c r="AC3" s="23"/>
-      <c r="AD3" s="23"/>
-      <c r="AE3" s="23"/>
-      <c r="AF3" s="23"/>
-      <c r="AG3" s="23"/>
-      <c r="AH3" s="23"/>
-      <c r="AI3" s="23"/>
-      <c r="AJ3" s="23"/>
-      <c r="AK3" s="23"/>
-      <c r="AL3" s="23"/>
-      <c r="AM3" s="23"/>
-      <c r="AN3" s="23"/>
-      <c r="AO3" s="23"/>
-      <c r="AP3" s="23"/>
-      <c r="AQ3" s="23"/>
-      <c r="AR3" s="23"/>
-      <c r="AS3" s="23"/>
-      <c r="AT3" s="23"/>
-      <c r="AU3" s="23"/>
-      <c r="AV3" s="23"/>
-      <c r="AW3" s="23"/>
-      <c r="AX3" s="23"/>
-      <c r="AY3" s="23"/>
-      <c r="AZ3" s="23"/>
-      <c r="BA3" s="23"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="22"/>
+      <c r="Q3" s="22"/>
+      <c r="R3" s="22"/>
+      <c r="S3" s="22"/>
+      <c r="T3" s="22"/>
+      <c r="U3" s="22"/>
+      <c r="V3" s="22"/>
+      <c r="W3" s="22"/>
+      <c r="X3" s="22"/>
+      <c r="Y3" s="22"/>
+      <c r="Z3" s="22"/>
+      <c r="AA3" s="22"/>
+      <c r="AB3" s="22"/>
+      <c r="AC3" s="22"/>
+      <c r="AD3" s="22"/>
+      <c r="AE3" s="22"/>
+      <c r="AF3" s="22"/>
+      <c r="AG3" s="22"/>
+      <c r="AH3" s="22"/>
+      <c r="AI3" s="22"/>
+      <c r="AJ3" s="22"/>
+      <c r="AK3" s="22"/>
+      <c r="AL3" s="22"/>
+      <c r="AM3" s="22"/>
+      <c r="AN3" s="22"/>
+      <c r="AO3" s="22"/>
+      <c r="AP3" s="22"/>
+      <c r="AQ3" s="22"/>
+      <c r="AR3" s="22"/>
+      <c r="AS3" s="22"/>
+      <c r="AT3" s="22"/>
+      <c r="AU3" s="22"/>
+      <c r="AV3" s="22"/>
+      <c r="AW3" s="22"/>
+      <c r="AX3" s="22"/>
+      <c r="AY3" s="22"/>
+      <c r="AZ3" s="22"/>
+      <c r="BA3" s="22"/>
     </row>
     <row r="4" spans="1:53" ht="14.4" x14ac:dyDescent="0.2">
-      <c r="A4" s="24"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="25"/>
-      <c r="K4" s="25"/>
-      <c r="L4" s="25"/>
-      <c r="M4" s="25"/>
-      <c r="N4" s="25"/>
-      <c r="O4" s="25"/>
-      <c r="P4" s="25"/>
-      <c r="Q4" s="25"/>
-      <c r="R4" s="25"/>
-      <c r="S4" s="25"/>
-      <c r="T4" s="25"/>
-      <c r="U4" s="25"/>
-      <c r="V4" s="25"/>
-      <c r="W4" s="25"/>
-      <c r="X4" s="25"/>
-      <c r="Y4" s="25"/>
-      <c r="Z4" s="25"/>
-      <c r="AA4" s="25"/>
-      <c r="AB4" s="25"/>
-      <c r="AC4" s="25"/>
-      <c r="AD4" s="25"/>
-      <c r="AE4" s="25"/>
-      <c r="AF4" s="25"/>
-      <c r="AG4" s="25"/>
-      <c r="AH4" s="25"/>
-      <c r="AI4" s="25"/>
-      <c r="AJ4" s="25"/>
-      <c r="AK4" s="25"/>
-      <c r="AL4" s="25"/>
-      <c r="AM4" s="25"/>
-      <c r="AN4" s="25"/>
-      <c r="AO4" s="25"/>
-      <c r="AP4" s="25"/>
-      <c r="AQ4" s="25"/>
-      <c r="AR4" s="25"/>
-      <c r="AS4" s="25"/>
-      <c r="AT4" s="25"/>
-      <c r="AU4" s="25"/>
-      <c r="AV4" s="25"/>
-      <c r="AW4" s="25"/>
-      <c r="AX4" s="25"/>
-      <c r="AY4" s="25"/>
-      <c r="AZ4" s="25"/>
-      <c r="BA4" s="25"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="24"/>
+      <c r="N4" s="24"/>
+      <c r="O4" s="24"/>
+      <c r="P4" s="24"/>
+      <c r="Q4" s="24"/>
+      <c r="R4" s="24"/>
+      <c r="S4" s="24"/>
+      <c r="T4" s="24"/>
+      <c r="U4" s="24"/>
+      <c r="V4" s="24"/>
+      <c r="W4" s="24"/>
+      <c r="X4" s="24"/>
+      <c r="Y4" s="24"/>
+      <c r="Z4" s="24"/>
+      <c r="AA4" s="24"/>
+      <c r="AB4" s="24"/>
+      <c r="AC4" s="24"/>
+      <c r="AD4" s="24"/>
+      <c r="AE4" s="24"/>
+      <c r="AF4" s="24"/>
+      <c r="AG4" s="24"/>
+      <c r="AH4" s="24"/>
+      <c r="AI4" s="24"/>
+      <c r="AJ4" s="24"/>
+      <c r="AK4" s="24"/>
+      <c r="AL4" s="24"/>
+      <c r="AM4" s="24"/>
+      <c r="AN4" s="24"/>
+      <c r="AO4" s="24"/>
+      <c r="AP4" s="24"/>
+      <c r="AQ4" s="24"/>
+      <c r="AR4" s="24"/>
+      <c r="AS4" s="24"/>
+      <c r="AT4" s="24"/>
+      <c r="AU4" s="24"/>
+      <c r="AV4" s="24"/>
+      <c r="AW4" s="24"/>
+      <c r="AX4" s="24"/>
+      <c r="AY4" s="24"/>
+      <c r="AZ4" s="24"/>
+      <c r="BA4" s="24"/>
     </row>
     <row r="5" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
@@ -2410,9 +2402,6 @@
       <c r="BA5" s="7" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="18" spans="29:29" x14ac:dyDescent="0.2">
-      <c r="AC18" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>